<commit_message>
push local changes and add published folder
</commit_message>
<xml_diff>
--- a/meta/procedure.xlsx
+++ b/meta/procedure.xlsx
@@ -10,7 +10,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhhW+ktJ/CDf7E+Uhu0IY6pgY/jjQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mi1OJmdOQJyLQep8jNgMRDn6dGGeA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -57,7 +57,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhvpPhfVIPv68J5M1GX3odDpbmMQQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miMaoPh7tvP97mMJAnfD9+Ed0wwFA=="/>
     </ext>
   </extLst>
 </comments>
@@ -138,14 +138,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjrewgim9B9Ix9l/es8+K4Mt4Sg+w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mibkeSnX9diq8vaVRzMeRIgYus9uw=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
   <si>
     <t>Part</t>
   </si>
@@ -381,16 +381,21 @@
     <t xml:space="preserve">Students learn new vocabulary. Then histogram is explained through a real world example of heights of cherry trees. </t>
   </si>
   <si>
-    <t xml:space="preserve">data visualization= 
-histogram= 
-bins=
-range= </t>
+    <t>analyzing= organizing and exploring data to unlock its meaning
+data visualization= a representation of numbers or other types of data in a way that makes it easier to see patterns. Ex: scatter plots, histograms, &amp; other types of graph
+range=a set of two numbers: the least and the greatest number in a data set. Usually expressed as Small Number – Big Number</t>
   </si>
   <si>
     <t>Concept: Dot Plot</t>
   </si>
   <si>
     <t>Students follow along as the presentation shows how the data is used to create a Dot Plot. Check-in formative assessments of understanding are built in.</t>
+  </si>
+  <si>
+    <t>dot plot= a graph with one point for each data observation
+binned dot plot= a dot plot where observations have been binned into ranges
+histogram= a type of bar graph showing the distribution of a set of measurements for 1 variable. A common pattern (called a "normal distribution") is bell-shaped, with most observations having values close to the average, with about equal, increasingly rare measurements that are very high or very low. Human height is a good example of a normal distribution, with many "average/medium" height individuals, and very few individuals being significantly shorter or taller than all the rest.
+scatter plot= a graph showing the relationship between two continuous variables. Each data point represents the measurement for variable X and variable Y for a particular individual.</t>
   </si>
   <si>
     <t>Concept: Binning</t>
@@ -400,6 +405,9 @@
   </si>
   <si>
     <t>This video has some silly sound effects which will hopefully increase engagement and help students remember the connections between dot plots and histograms.</t>
+  </si>
+  <si>
+    <t>binning= combining groups of observations into ranges. The bins could be ranges (like 0-5, 6-10, etc), or named categories, like when we classify people into “short,” “average,” and “tall” height categories.</t>
   </si>
   <si>
     <t>Synthesis</t>
@@ -433,7 +441,7 @@
     <t>Warm-Up &amp; Review</t>
   </si>
   <si>
-    <t>Students warm up with a cipher. They need to shift back 3 to decipher “FEMALES SING,” referring to the overlooked fact that many species of birds sing, just less frequently than males.</t>
+    <t>Students warm up with a cipher. They need to shift back 3 to decipher “FEMALES SING,” referring to the overlooked fact that females in many bird species sing, just less frequently than males.</t>
   </si>
   <si>
     <t>Make sure to only spend a few minutes on the warm-up. This is a long lesson.</t>
@@ -449,6 +457,10 @@
   </si>
   <si>
     <t>Students are guided through understanding what the data are and how they are categorized in Table 1. This is the raw data, representing the number of songs recorded for each bird, along with their sex &amp; ID code.</t>
+  </si>
+  <si>
+    <t>binned data= summary data where measurements have been combined into bins (ranges)
+raw data= original, unmodified measurements</t>
   </si>
   <si>
     <t>Connecting the Data to Reality</t>
@@ -813,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -892,6 +904,9 @@
     </xf>
     <xf borderId="13" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10299,7 +10314,7 @@
     <col customWidth="1" min="4" max="4" width="12.86"/>
     <col customWidth="1" min="5" max="5" width="5.29"/>
     <col customWidth="1" min="6" max="6" width="14.14"/>
-    <col customWidth="1" min="7" max="7" width="22.29"/>
+    <col customWidth="1" min="7" max="7" width="25.86"/>
     <col customWidth="1" min="8" max="8" width="43.43"/>
     <col customWidth="1" min="9" max="9" width="30.71"/>
     <col customWidth="1" min="10" max="10" width="35.29"/>
@@ -10847,7 +10862,9 @@
         <v>76</v>
       </c>
       <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
+      <c r="I14" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
       <c r="M14" s="23"/>
@@ -10872,15 +10889,17 @@
         <v>5.0</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="26"/>
+        <v>80</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>81</v>
+      </c>
       <c r="J15" s="26"/>
       <c r="K15" s="26"/>
       <c r="M15" s="23"/>
@@ -10903,16 +10922,16 @@
         <v>10.0</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E16" s="26">
         <v>6.0</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
@@ -10938,7 +10957,7 @@
         <v>5.0</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E17" s="26">
         <v>7.0</v>
@@ -10947,7 +10966,7 @@
         <v>69</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
@@ -10975,18 +10994,18 @@
         <v>8.0</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="26" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M18" s="23"/>
       <c r="N18" s="24"/>
@@ -11008,7 +11027,7 @@
         <v>5.0</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E19" s="26">
         <v>1.0</v>
@@ -11016,14 +11035,14 @@
       <c r="F19" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="28" t="s">
-        <v>90</v>
+      <c r="G19" s="31" t="s">
+        <v>92</v>
       </c>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
       <c r="J19" s="26"/>
       <c r="K19" s="26" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M19" s="23"/>
       <c r="N19" s="24"/>
@@ -11050,7 +11069,7 @@
         <v>69</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
@@ -11076,19 +11095,21 @@
         <v>10.0</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E21" s="26">
         <v>3.0</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
+      <c r="I21" s="26" t="s">
+        <v>98</v>
+      </c>
       <c r="J21" s="26"/>
       <c r="K21" s="26"/>
       <c r="M21" s="23"/>
@@ -11113,10 +11134,10 @@
         <v>4.0</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
@@ -11144,10 +11165,10 @@
         <v>5.0</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
@@ -11173,16 +11194,16 @@
         <v>10.0</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E24" s="26">
         <v>6.0</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H24" s="26"/>
       <c r="I24" s="26"/>
@@ -11210,10 +11231,10 @@
         <v>7.0</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
@@ -11241,15 +11262,15 @@
         <v>8.0</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="29"/>
       <c r="J26" s="29" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K26" s="26"/>
       <c r="M26" s="23"/>
@@ -11272,24 +11293,24 @@
         <v>5.0</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E27" s="26">
         <v>9.0</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I27" s="26"/>
       <c r="J27" s="26"/>
       <c r="K27" s="26" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="M27" s="23"/>
       <c r="N27" s="24"/>
@@ -11311,24 +11332,24 @@
         <v>5.0</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E28" s="26">
         <v>10.0</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
       <c r="J28" s="26" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="K28" s="26" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M28" s="23"/>
       <c r="N28" s="24"/>
@@ -11350,16 +11371,16 @@
         <v>10.0</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E29" s="26">
         <v>11.0</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
@@ -11390,12 +11411,12 @@
         <v>62</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
       <c r="J30" s="26" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="K30" s="26"/>
       <c r="M30" s="23"/>
@@ -11420,16 +11441,16 @@
         <v>13.0</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G31" s="28" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
       <c r="J31" s="26"/>
       <c r="K31" s="26" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="M31" s="23"/>
       <c r="N31" s="24"/>

</xml_diff>